<commit_message>
Check sealevel conversion. Looks good
</commit_message>
<xml_diff>
--- a/LakeLevelAnalysis.xlsx
+++ b/LakeLevelAnalysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91F2A92-5E00-49D8-9D15-075AFFA25577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53B62C8-D937-4420-AED7-18D9353578BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29920" yWindow="1270" windowWidth="28800" windowHeight="15410" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="24" yWindow="744" windowWidth="23016" windowHeight="12216" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="6" r:id="rId1"/>
@@ -29,8 +29,8 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="19" r:id="rId7"/>
-    <pivotCache cacheId="23" r:id="rId8"/>
+    <pivotCache cacheId="24" r:id="rId7"/>
+    <pivotCache cacheId="25" r:id="rId8"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -86,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>FROM:</t>
   </si>
@@ -284,6 +284,9 @@
   </si>
   <si>
     <t>Range</t>
+  </si>
+  <si>
+    <t>I checked my conversion with that of the state. Looks like I got it correct.</t>
   </si>
 </sst>
 </file>
@@ -533,7 +536,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -566,7 +569,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -584,9 +586,12 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="26">
     <dxf>
-      <alignment horizontal="center"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -599,15 +604,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <alignment horizontal="center"/>
@@ -844,27 +840,27 @@
   </dxfs>
   <tableStyles count="2" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Standard Pivot Table" table="0" count="12" xr9:uid="{94886349-6B4A-4300-89B0-9F83C8B5183A}">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="totalRow" dxfId="25"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="24"/>
-      <tableStyleElement type="firstHeaderCell" dxfId="23"/>
-      <tableStyleElement type="firstSubtotalColumn" dxfId="22"/>
-      <tableStyleElement type="firstSubtotalRow" dxfId="21"/>
-      <tableStyleElement type="secondSubtotalRow" dxfId="20"/>
-      <tableStyleElement type="firstRowSubheading" dxfId="19"/>
-      <tableStyleElement type="secondRowSubheading" dxfId="18"/>
-      <tableStyleElement type="pageFieldLabels" dxfId="17"/>
-      <tableStyleElement type="pageFieldValues" dxfId="16"/>
+      <tableStyleElement type="wholeTable" dxfId="25"/>
+      <tableStyleElement type="headerRow" dxfId="24"/>
+      <tableStyleElement type="totalRow" dxfId="23"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="22"/>
+      <tableStyleElement type="firstHeaderCell" dxfId="21"/>
+      <tableStyleElement type="firstSubtotalColumn" dxfId="20"/>
+      <tableStyleElement type="firstSubtotalRow" dxfId="19"/>
+      <tableStyleElement type="secondSubtotalRow" dxfId="18"/>
+      <tableStyleElement type="firstRowSubheading" dxfId="17"/>
+      <tableStyleElement type="secondRowSubheading" dxfId="16"/>
+      <tableStyleElement type="pageFieldLabels" dxfId="15"/>
+      <tableStyleElement type="pageFieldValues" dxfId="14"/>
     </tableStyle>
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="15"/>
-      <tableStyleElement type="headerRow" dxfId="14"/>
-      <tableStyleElement type="totalRow" dxfId="13"/>
-      <tableStyleElement type="firstColumn" dxfId="12"/>
-      <tableStyleElement type="lastColumn" dxfId="11"/>
-      <tableStyleElement type="firstRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -15358,8 +15354,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="158750" y="0"/>
-          <a:ext cx="2206625" cy="495300"/>
+          <a:off x="160020" y="0"/>
+          <a:ext cx="2206625" cy="502920"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="512657"/>
         </a:xfrm>
@@ -15772,7 +15768,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Append1!$G$1:$P$19" spid="_x0000_s2079"/>
+                  <a14:cameraTool cellRange="Append1!$G$1:$P$19" spid="_x0000_s2082"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -15908,7 +15904,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Append1!$R$1:$AA$19" spid="_x0000_s2080"/>
+                  <a14:cameraTool cellRange="Append1!$R$1:$AA$19" spid="_x0000_s2083"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -15972,7 +15968,7 @@
               <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
               <a:extLst>
                 <a:ext uri="{84589F7E-364E-4C9E-8A38-B11213B215E9}">
-                  <a14:cameraTool cellRange="Sheet1!$G$4:$I$10" spid="_x0000_s2081"/>
+                  <a14:cameraTool cellRange="Sheet1!$G$4:$I$10" spid="_x0000_s2084"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPicPr>
@@ -16155,8 +16151,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3190241" y="255215"/>
-          <a:ext cx="2197735" cy="450270"/>
+          <a:off x="3187701" y="260295"/>
+          <a:ext cx="2195195" cy="456620"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -19176,7 +19172,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{006C83EF-0D39-43D0-B76F-B6FCA3AFEA23}" name="PivotTable1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{006C83EF-0D39-43D0-B76F-B6FCA3AFEA23}" name="PivotTable1" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" showDrill="0" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B3:D27" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" compact="0" numFmtId="14" subtotalTop="0" showAll="0" defaultSubtotal="0">
@@ -19862,7 +19858,7 @@
     <dataField name="Max Level (ft)" fld="1" subtotal="max" baseField="4" baseItem="1" numFmtId="2"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="8">
+    <format dxfId="6">
       <pivotArea dataOnly="0" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
@@ -19879,7 +19875,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="19" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -19994,8 +19990,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{3DE390EC-C374-4B25-A1D3-3088DB991017}" name="Append1" displayName="Append1" ref="A1:B544" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B544" xr:uid="{3DE390EC-C374-4B25-A1D3-3088DB991017}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{34F7F1E8-8FC8-4FA0-ADD2-BBC9197CA2F3}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{53F079B8-251E-489B-A10A-E8925BCECD4F}" uniqueName="2" name="Sealevel" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{34F7F1E8-8FC8-4FA0-ADD2-BBC9197CA2F3}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{53F079B8-251E-489B-A10A-E8925BCECD4F}" uniqueName="2" name="Sealevel" queryTableFieldId="2" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -20005,7 +20001,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{98F2B62E-4934-422A-99A0-FE071B4B285F}" name="NewData_1" displayName="NewData_1" ref="A1:B2" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:B2" xr:uid="{98F2B62E-4934-422A-99A0-FE071B4B285F}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{99C1AC08-A55B-469A-8C61-F5AC5C79FCD6}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{99C1AC08-A55B-469A-8C61-F5AC5C79FCD6}" uniqueName="1" name="Date" queryTableFieldId="1" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{B78903B8-431B-4DB7-BBA2-CC37BDF4AF38}" uniqueName="2" name="Sealevel" queryTableFieldId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -20016,9 +20012,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{BD04B1ED-0E94-41A6-9A23-75D8C75231F4}" name="NewData" displayName="NewData" ref="F1:H2" totalsRowShown="0">
   <autoFilter ref="F1:H2" xr:uid="{BD04B1ED-0E94-41A6-9A23-75D8C75231F4}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6D60DF79-FCF3-4ECC-AF69-F7B7EB2F5316}" name="Date" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{E01C1CBF-5C61-426E-8D72-F1835B019727}" name="Reading" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{478D1094-8F68-4899-A317-69309383F693}" name="Sealevel" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{6D60DF79-FCF3-4ECC-AF69-F7B7EB2F5316}" name="Date" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E01C1CBF-5C61-426E-8D72-F1835B019727}" name="Reading" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{478D1094-8F68-4899-A317-69309383F693}" name="Sealevel" dataDxfId="0">
       <calculatedColumnFormula>NewData[[#This Row],[Reading]]+Datum</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -20539,7 +20535,7 @@
   <dimension ref="A1:J544"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -20709,6 +20705,9 @@
       </c>
       <c r="B19" s="10">
         <v>1376.63</v>
+      </c>
+      <c r="G19" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -25855,7 +25854,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-Jul-2024</v>
+        <v>23-Jul-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -25991,19 +25990,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -26011,11 +26006,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="24"/>
-      <c r="E21" s="24">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="24">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -26023,19 +26017,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="24">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -26043,11 +26033,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="24"/>
-      <c r="E24" s="24">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="24">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -26055,19 +26044,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="24">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -26075,11 +26060,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="24"/>
-      <c r="E27" s="24">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="24">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -26087,13 +26071,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="24">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="24">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="24">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -26166,7 +26150,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>22-Jul-2024</v>
+        <v>23-Jul-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>